<commit_message>
modify milestones and game ideas
</commit_message>
<xml_diff>
--- a/Milestones and work done.xlsx
+++ b/Milestones and work done.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TP\Documents\Nolan Chappuis\VR_GAME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C9B99E9C-89E9-44A5-B35E-220AF829384C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C93AEB-EDCC-4C49-A292-C71A41EAF32F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C1D227EA-EE83-4B9B-A096-469D711968A3}"/>
   </bookViews>
@@ -97,15 +97,14 @@
 change things if needed</t>
   </si>
   <si>
-    <t>Test the final, get feedback, solve potential flows and
-change things if needed</t>
-  </si>
-  <si>
     <t>Week 15</t>
   </si>
   <si>
     <t>Implement various trigger mechanisms and needed
 features</t>
+  </si>
+  <si>
+    <t>Test the final product, get feedback, solve potential flows and change things if needed</t>
   </si>
 </sst>
 </file>
@@ -605,7 +604,7 @@
   <dimension ref="D1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5"/>
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -665,7 +664,7 @@
       </c>
       <c r="E5" s="2"/>
       <c r="G5" s="15" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H5" s="8" t="s">
         <v>10</v>
@@ -737,10 +736,10 @@
       </c>
       <c r="E11" s="10"/>
       <c r="G11" s="16" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="9" t="s">
         <v>21</v>
-      </c>
-      <c r="H11" s="9" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="12" spans="4:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
week 02 work done
</commit_message>
<xml_diff>
--- a/Milestones and work done.xlsx
+++ b/Milestones and work done.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TP\Documents\Nolan Chappuis\VR_GAME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C93AEB-EDCC-4C49-A292-C71A41EAF32F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DBD5EB-738F-46BA-A54C-9853E82DEF73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C1D227EA-EE83-4B9B-A096-469D711968A3}"/>
   </bookViews>
@@ -36,10 +36,6 @@
     <t>Game plan &amp; familiarize with new work station</t>
   </si>
   <si>
-    <t>Set up git, create project with basic scene, familirize with 
-Unity Steam VR implementation</t>
-  </si>
-  <si>
     <t>Milestones</t>
   </si>
   <si>
@@ -105,6 +101,10 @@
   </si>
   <si>
     <t>Test the final product, get feedback, solve potential flows and change things if needed</t>
+  </si>
+  <si>
+    <t>Set up git, create project with basic scene, familirize with 
+Unity Steam VR implementation, implement grabbing</t>
   </si>
 </sst>
 </file>
@@ -604,7 +604,7 @@
   <dimension ref="D1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -624,10 +624,10 @@
         <v>1</v>
       </c>
       <c r="G2" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="H2" s="5" t="s">
         <v>4</v>
-      </c>
-      <c r="H2" s="5" t="s">
-        <v>5</v>
       </c>
     </row>
     <row r="3" spans="4:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -638,10 +638,10 @@
         <v>2</v>
       </c>
       <c r="G3" s="14" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H3" s="8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4" spans="4:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -649,13 +649,13 @@
         <v>2</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>3</v>
+        <v>23</v>
       </c>
       <c r="G4" s="14" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H4" s="8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="4:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -664,10 +664,10 @@
       </c>
       <c r="E5" s="2"/>
       <c r="G5" s="15" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="4:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -676,10 +676,10 @@
       </c>
       <c r="E6" s="10"/>
       <c r="G6" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>11</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7" spans="4:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -688,10 +688,10 @@
       </c>
       <c r="E7" s="10"/>
       <c r="G7" s="15" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="4:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -700,10 +700,10 @@
       </c>
       <c r="E8" s="10"/>
       <c r="G8" s="15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="9" spans="4:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -712,10 +712,10 @@
       </c>
       <c r="E9" s="10"/>
       <c r="G9" s="15" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="10" spans="4:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -724,10 +724,10 @@
       </c>
       <c r="E10" s="10"/>
       <c r="G10" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H10" s="8" t="s">
         <v>18</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="11" spans="4:8" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -736,10 +736,10 @@
       </c>
       <c r="E11" s="10"/>
       <c r="G11" s="16" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="12" spans="4:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
modify week 03 milestones
</commit_message>
<xml_diff>
--- a/Milestones and work done.xlsx
+++ b/Milestones and work done.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TP\Documents\Nolan Chappuis\VR_GAME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94DBD5EB-738F-46BA-A54C-9853E82DEF73}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F5CBAE1-A806-4681-964E-28360F7A834B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C1D227EA-EE83-4B9B-A096-469D711968A3}"/>
   </bookViews>
@@ -51,9 +51,6 @@
     <t>Week 03</t>
   </si>
   <si>
-    <t>Implement and test Infinadeck with Unity (need 2 person)</t>
-  </si>
-  <si>
     <t>Week 03-06</t>
   </si>
   <si>
@@ -105,6 +102,10 @@
   <si>
     <t>Set up git, create project with basic scene, familirize with 
 Unity Steam VR implementation, implement grabbing</t>
+  </si>
+  <si>
+    <t>Implement and test Infinadeck with Unity (need 2 person)
+&amp; change inputs to walk with controllers</t>
   </si>
 </sst>
 </file>
@@ -604,7 +605,7 @@
   <dimension ref="D1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="M7" sqref="M7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -649,10 +650,10 @@
         <v>2</v>
       </c>
       <c r="E4" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="G4" s="15" t="s">
         <v>23</v>
-      </c>
-      <c r="G4" s="14" t="s">
-        <v>8</v>
       </c>
       <c r="H4" s="8" t="s">
         <v>7</v>
@@ -664,10 +665,10 @@
       </c>
       <c r="E5" s="2"/>
       <c r="G5" s="15" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="6" spans="4:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -676,10 +677,10 @@
       </c>
       <c r="E6" s="10"/>
       <c r="G6" s="15" t="s">
+        <v>9</v>
+      </c>
+      <c r="H6" s="8" t="s">
         <v>10</v>
-      </c>
-      <c r="H6" s="8" t="s">
-        <v>11</v>
       </c>
     </row>
     <row r="7" spans="4:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -688,10 +689,10 @@
       </c>
       <c r="E7" s="10"/>
       <c r="G7" s="15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="H7" s="8" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="8" spans="4:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -700,10 +701,10 @@
       </c>
       <c r="E8" s="10"/>
       <c r="G8" s="15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="4:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -712,10 +713,10 @@
       </c>
       <c r="E9" s="10"/>
       <c r="G9" s="15" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H9" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="10" spans="4:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -724,10 +725,10 @@
       </c>
       <c r="E10" s="10"/>
       <c r="G10" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="8" t="s">
         <v>17</v>
-      </c>
-      <c r="H10" s="8" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="4:8" ht="43.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -736,10 +737,10 @@
       </c>
       <c r="E11" s="10"/>
       <c r="G11" s="16" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="12" spans="4:8" ht="43.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Update milestones and work done
</commit_message>
<xml_diff>
--- a/Milestones and work done.xlsx
+++ b/Milestones and work done.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TP\Documents\Nolan Chappuis\VR_GAME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B217FA18-9B35-4163-B7ED-B4974A97D5BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0FB2088-64AB-4BE5-B880-6A3A47D5CF9A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C1D227EA-EE83-4B9B-A096-469D711968A3}"/>
   </bookViews>
@@ -115,7 +115,7 @@
 features, writing with voice off, first design</t>
   </si>
   <si>
-    <t>Correct drawers &amp; doors, create own key, start tutorial and story writing</t>
+    <t>Correct drawers &amp; doors, create own key, start tutorial and story writing, improve lock and keys, key animation</t>
   </si>
 </sst>
 </file>
@@ -617,7 +617,7 @@
   <dimension ref="D1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Update work done for week 9
</commit_message>
<xml_diff>
--- a/Milestones and work done.xlsx
+++ b/Milestones and work done.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20384"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20385"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TP\Documents\Nolan Chappuis\VR_GAME\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C959A07C-3C2A-44CE-9AE4-5F2EB87E9B20}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CAA5BCB-4B58-4FB7-8A20-0739C437559C}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C1D227EA-EE83-4B9B-A096-469D711968A3}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>Week</t>
   </si>
@@ -131,6 +131,9 @@
   </si>
   <si>
     <t>https://assetstore.unity.com/packages/audio/sound-fx/complete-survival-game-sound-kit-159941</t>
+  </si>
+  <si>
+    <t>Objects can't fall to the ground, level 1 design first draft, creation of level 1 puzzles</t>
   </si>
 </sst>
 </file>
@@ -645,7 +648,7 @@
   <dimension ref="D1:H17"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="K13" sqref="K13"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -773,7 +776,9 @@
       <c r="D10" s="2">
         <v>8</v>
       </c>
-      <c r="E10" s="5"/>
+      <c r="E10" s="5" t="s">
+        <v>32</v>
+      </c>
       <c r="G10" s="11" t="s">
         <v>13</v>
       </c>
@@ -785,7 +790,6 @@
       <c r="D11" s="2">
         <v>9</v>
       </c>
-      <c r="E11" s="5"/>
       <c r="G11" s="12" t="s">
         <v>22</v>
       </c>

</xml_diff>